<commit_message>
adds JPR to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45103DEF-9EA4-462B-85B9-D283CA7BC009}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="1170" yWindow="795" windowWidth="31275" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="174">
   <si>
     <t>*N/A*</t>
   </si>
@@ -552,6 +552,12 @@
   </si>
   <si>
     <t>3.5k -- 6.5k words</t>
+  </si>
+  <si>
+    <t>Journal of Peace Research</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.prio.org/journals/jpr/submissions'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -923,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1037,27 +1043,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" t="s">
-        <v>131</v>
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
         <v>131</v>
@@ -1065,13 +1071,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="D10" t="s">
         <v>131</v>
@@ -1079,13 +1085,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
         <v>131</v>
@@ -1093,27 +1099,27 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
         <v>135</v>
@@ -1121,55 +1127,55 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
         <v>140</v>
@@ -1177,27 +1183,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
         <v>141</v>
@@ -1205,30 +1211,30 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1236,7 +1242,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
         <v>143</v>
@@ -1247,27 +1253,27 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D24" t="s">
         <v>146</v>
@@ -1275,13 +1281,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
         <v>146</v>
@@ -1292,10 +1298,10 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="D26" t="s">
         <v>146</v>
@@ -1303,27 +1309,27 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
         <v>149</v>
@@ -1331,27 +1337,27 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D30" t="s">
         <v>152</v>
@@ -1359,55 +1365,55 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="D34" t="s">
         <v>156</v>
@@ -1415,13 +1421,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D35" t="s">
         <v>156</v>
@@ -1429,41 +1435,41 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D38" t="s">
         <v>158</v>
@@ -1471,27 +1477,27 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
         <v>159</v>
@@ -1499,13 +1505,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D41" t="s">
         <v>159</v>
@@ -1513,24 +1519,24 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
         <v>136</v>
@@ -1541,27 +1547,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
         <v>162</v>
@@ -1569,41 +1575,41 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
         <v>165</v>
@@ -1611,27 +1617,27 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C49" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
         <v>166</v>
@@ -1639,69 +1645,69 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C53" t="s">
         <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="D55" t="s">
         <v>0</v>
@@ -1709,13 +1715,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
         <v>0</v>
@@ -1723,13 +1729,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
         <v>0</v>
@@ -1737,10 +1743,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
         <v>128</v>
@@ -1751,21 +1757,35 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D59" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D53">
-    <sortCondition descending="1" ref="D2:D53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
+    <sortCondition descending="1" ref="D2:D54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds JoDemocracy to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45103DEF-9EA4-462B-85B9-D283CA7BC009}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{559FE356-C2BE-4591-B627-631F7DB84B8A}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="795" windowWidth="31275" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="1560" yWindow="795" windowWidth="31275" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="176">
   <si>
     <t>*N/A*</t>
   </si>
@@ -558,6 +558,12 @@
   </si>
   <si>
     <t>&lt;a href='https://www.prio.org/journals/jpr/submissions'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Journal of Democracy</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.journalofdemocracy.org/about/submissions/'target='_blank'&gt;Online Exclusive&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -610,6 +616,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -929,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1057,27 +1067,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" t="s">
-        <v>131</v>
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
         <v>131</v>
@@ -1085,13 +1095,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="D11" t="s">
         <v>131</v>
@@ -1099,13 +1109,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
         <v>131</v>
@@ -1113,27 +1123,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
         <v>135</v>
@@ -1141,55 +1151,55 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
         <v>140</v>
@@ -1197,27 +1207,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
         <v>141</v>
@@ -1225,30 +1235,30 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,7 +1266,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
         <v>143</v>
@@ -1267,27 +1277,27 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
         <v>146</v>
@@ -1295,13 +1305,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
         <v>146</v>
@@ -1312,10 +1322,10 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
         <v>146</v>
@@ -1323,27 +1333,27 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D29" t="s">
         <v>149</v>
@@ -1351,27 +1361,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D31" t="s">
         <v>152</v>
@@ -1379,55 +1389,55 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
         <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="D35" t="s">
         <v>156</v>
@@ -1435,13 +1445,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s">
         <v>156</v>
@@ -1449,41 +1459,41 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D39" t="s">
         <v>158</v>
@@ -1491,27 +1501,27 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
         <v>159</v>
@@ -1519,13 +1529,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D42" t="s">
         <v>159</v>
@@ -1533,24 +1543,24 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
         <v>136</v>
@@ -1561,27 +1571,27 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="D45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="D46" t="s">
         <v>162</v>
@@ -1589,41 +1599,41 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="D49" t="s">
         <v>165</v>
@@ -1631,27 +1641,27 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
         <v>166</v>
@@ -1659,69 +1669,69 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C54" t="s">
         <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
         <v>0</v>
@@ -1729,13 +1739,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="D57" t="s">
         <v>0</v>
@@ -1743,13 +1753,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
         <v>0</v>
@@ -1757,10 +1767,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
         <v>128</v>
@@ -1771,21 +1781,35 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="C60" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D60" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
-    <sortCondition descending="1" ref="D2:D54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D55">
+    <sortCondition descending="1" ref="D2:D55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds journals and footnotes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{559FE356-C2BE-4591-B627-631F7DB84B8A}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53EBE123-F70F-2840-9780-C022ACF55BF2}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="795" windowWidth="31275" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="18420" yWindow="500" windowWidth="31280" windowHeight="20800" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="180">
   <si>
     <t>*N/A*</t>
   </si>
@@ -564,6 +564,18 @@
   </si>
   <si>
     <t>&lt;a href='https://www.journalofdemocracy.org/about/submissions/'target='_blank'&gt;Online Exclusive&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Acta Politica</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.palgrave.com/gp/journal/41269/authors/submission'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Australian Journal of Public Administration</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://onlinelibrary.wiley.com/page/journal/14678500/homepage/forauthors.html'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -616,10 +628,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -939,21 +947,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
-    <col min="2" max="2" width="135.375" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="135.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -967,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -981,7 +989,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -995,7 +1003,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1017,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1023,7 +1031,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1051,7 +1059,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -1065,7 +1073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1101,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1107,7 +1115,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1121,7 +1129,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1171,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1177,7 +1185,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1191,7 +1199,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1205,7 +1213,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1219,7 +1227,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1261,7 +1269,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1275,7 +1283,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1289,7 +1297,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1303,7 +1311,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1317,7 +1325,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1331,7 +1339,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1345,7 +1353,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1359,7 +1367,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1373,7 +1381,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1409,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1415,7 +1423,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1443,7 +1451,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1457,7 +1465,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1471,306 +1479,306 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>97</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>143</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>98</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>132</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
       </c>
       <c r="C42" t="s">
         <v>128</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>46</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>103</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>136</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>104</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>136</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>105</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>161</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>106</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>0</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D49" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>50</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>107</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>163</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D50" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>108</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>145</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D51" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>52</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>109</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>128</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D52" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>110</v>
-      </c>
-      <c r="C51" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" t="s">
-        <v>112</v>
       </c>
       <c r="C53" t="s">
         <v>120</v>
       </c>
       <c r="D53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>113</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>134</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D56" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>57</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>114</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>134</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>58</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>115</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>170</v>
-      </c>
-      <c r="D56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" t="s">
-        <v>128</v>
-      </c>
-      <c r="D57" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" t="s">
-        <v>117</v>
-      </c>
-      <c r="C58" t="s">
-        <v>171</v>
       </c>
       <c r="D58" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
         <v>128</v>
@@ -1779,37 +1787,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="D60" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D61" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D55">
-    <sortCondition descending="1" ref="D2:D55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
+    <sortCondition descending="1" ref="D2:D57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds jpla to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53EBE123-F70F-2840-9780-C022ACF55BF2}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EBB57BE-1852-42B4-AD24-106C7F15DD8A}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="500" windowWidth="31280" windowHeight="20800" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="3630" yWindow="585" windowWidth="35925" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="182">
   <si>
     <t>*N/A*</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>&lt;a href='https://onlinelibrary.wiley.com/page/journal/14678500/homepage/forauthors.html'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Journal of Politics in Latin America</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://journals.sagepub.com/author-instructions/PLA'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -628,6 +634,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -947,21 +957,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="2" max="2" width="135.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="135.375" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -975,7 +985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -989,7 +999,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +1013,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1027,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1031,7 +1041,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1059,7 +1069,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -1073,7 +1083,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1087,7 +1097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1101,7 +1111,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1129,7 +1139,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1143,7 +1153,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1157,7 +1167,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1199,7 +1209,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1213,7 +1223,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1237,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1241,7 +1251,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1255,7 +1265,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1269,7 +1279,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1293,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1311,7 +1321,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1325,7 +1335,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1353,7 +1363,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1367,7 +1377,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1381,7 +1391,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1395,7 +1405,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1409,7 +1419,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1423,7 +1433,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1437,7 +1447,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1451,7 +1461,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1479,7 +1489,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -1493,7 +1503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>176</v>
       </c>
@@ -1507,7 +1517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1521,7 +1531,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1535,7 +1545,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1549,7 +1559,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1577,7 +1587,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1591,7 +1601,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1605,7 +1615,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1619,7 +1629,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1633,7 +1643,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1647,7 +1657,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1661,7 +1671,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1675,7 +1685,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1689,7 +1699,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1703,7 +1713,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1717,7 +1727,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1731,7 +1741,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1745,7 +1755,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1759,7 +1769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1773,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1787,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1801,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1815,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1829,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -1840,6 +1850,20 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds jitp to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBA7A682-E202-264B-8F1C-DFF7D3E6667B}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65684E99-12ED-4934-8A85-BD59EDEBA710}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="580" windowWidth="35920" windowHeight="20800" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="15000" yWindow="75" windowWidth="35925" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="184">
   <si>
     <t>*N/A*</t>
   </si>
@@ -582,6 +582,12 @@
   </si>
   <si>
     <t>&lt;a href='https://www.elevenjournals.com/tijdschrift/PLC/detail'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Journal of Information Technology &amp; Politics</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=witp20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -634,6 +640,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -953,21 +963,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="2" max="2" width="135.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="135.375" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -981,7 +991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -995,7 +1005,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1009,7 +1019,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +1033,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1061,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -1079,7 +1089,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1093,7 +1103,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1107,7 +1117,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1121,7 +1131,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1145,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1149,7 +1159,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1163,7 +1173,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1187,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1191,7 +1201,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1219,7 +1229,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1233,7 +1243,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1247,7 +1257,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1261,7 +1271,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1275,7 +1285,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1289,7 +1299,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1313,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1317,7 +1327,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1331,7 +1341,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1345,7 +1355,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1359,7 +1369,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1373,7 +1383,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1387,236 +1397,236 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>151</v>
-      </c>
-      <c r="D31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>132</v>
       </c>
       <c r="D32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>92</v>
-      </c>
-      <c r="C33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" t="s">
-        <v>93</v>
       </c>
       <c r="C34" t="s">
         <v>120</v>
       </c>
       <c r="D34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>94</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>155</v>
-      </c>
-      <c r="D35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" t="s">
-        <v>120</v>
       </c>
       <c r="D36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>178</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>179</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>139</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>176</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>177</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>0</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>97</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>143</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>98</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>132</v>
-      </c>
-      <c r="D41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
       </c>
       <c r="D42" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>100</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>136</v>
-      </c>
-      <c r="D43" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" t="s">
-        <v>128</v>
       </c>
       <c r="D44" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>103</v>
-      </c>
-      <c r="C46" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>104</v>
       </c>
       <c r="C47" t="s">
         <v>136</v>
@@ -1625,208 +1635,208 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>105</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>161</v>
-      </c>
-      <c r="D48" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" t="s">
-        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>107</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>163</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>108</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>145</v>
-      </c>
-      <c r="D51" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" t="s">
-        <v>128</v>
       </c>
       <c r="D52" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>110</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>120</v>
-      </c>
-      <c r="D53" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1</v>
       </c>
       <c r="D54" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>112</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>120</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>113</v>
-      </c>
-      <c r="C56" t="s">
-        <v>134</v>
-      </c>
-      <c r="D56" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" t="s">
-        <v>114</v>
       </c>
       <c r="C57" t="s">
         <v>134</v>
       </c>
       <c r="D57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
+        <v>134</v>
+      </c>
+      <c r="D58" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>115</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>170</v>
-      </c>
-      <c r="D58" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" t="s">
-        <v>128</v>
       </c>
       <c r="D59" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="D60" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="D61" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
         <v>128</v>
@@ -1835,37 +1845,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D63" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
-    <sortCondition descending="1" ref="D2:D57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">
+    <sortCondition descending="1" ref="D2:D58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds four journals to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65684E99-12ED-4934-8A85-BD59EDEBA710}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{633F962C-927E-F841-B471-016B58194CAD}"/>
   <bookViews>
-    <workbookView xWindow="15000" yWindow="75" windowWidth="35925" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="12780" yWindow="500" windowWidth="35920" windowHeight="20800" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
   <si>
     <t>*N/A*</t>
   </si>
@@ -588,6 +588,33 @@
   </si>
   <si>
     <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=witp20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Conflict Management and Peace Science</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://journals.sagepub.com/author-instructions/CMP'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Journal of East Asian Studies</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/journal-of-east-asian-studies/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Relations of the Asia-Pacific </t>
+  </si>
+  <si>
+    <t>10k words</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://academic.oup.com/irap/pages/General_Instructions'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal of Global Security Studies </t>
+  </si>
+  <si>
+    <t>&lt;a href='https://academic.oup.com/jogss/pages/General_Instructions'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -640,10 +667,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -963,21 +986,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
-    <col min="2" max="2" width="135.375" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="135.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -991,7 +1014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1028,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1042,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1056,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1047,7 +1070,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1084,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1075,7 +1098,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -1089,7 +1112,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1103,7 +1126,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1140,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1154,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1145,7 +1168,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1182,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1173,7 +1196,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1210,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1201,7 +1224,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1238,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1229,7 +1252,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1243,7 +1266,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1257,7 +1280,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1271,7 +1294,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1285,7 +1308,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1299,7 +1322,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1313,7 +1336,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1327,7 +1350,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1341,7 +1364,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1355,7 +1378,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +1392,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1383,7 +1406,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1397,7 +1420,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>182</v>
       </c>
@@ -1411,7 +1434,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1425,7 +1448,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1439,7 +1462,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1453,7 +1476,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1467,7 +1490,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1481,7 +1504,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1495,7 +1518,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1509,7 +1532,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -1523,7 +1546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>176</v>
       </c>
@@ -1537,7 +1560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1551,7 +1574,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1565,7 +1588,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1579,7 +1602,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1593,7 +1616,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1607,7 +1630,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1621,7 +1644,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1635,7 +1658,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1649,7 +1672,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1663,7 +1686,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1677,7 +1700,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1691,7 +1714,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1705,7 +1728,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1719,7 +1742,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1733,7 +1756,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1747,7 +1770,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1761,7 +1784,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1775,7 +1798,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1789,7 +1812,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1803,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1817,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1831,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1845,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1859,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -1873,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>180</v>
       </c>
@@ -1885,6 +1908,62 @@
       </c>
       <c r="D65" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>186</v>
+      </c>
+      <c r="B67" t="s">
+        <v>187</v>
+      </c>
+      <c r="C67" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" t="s">
+        <v>189</v>
+      </c>
+      <c r="D68">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>191</v>
+      </c>
+      <c r="B69" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds SPPQ to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{633F962C-927E-F841-B471-016B58194CAD}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2008722D-8A2D-4A31-8080-3248B042069E}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="500" windowWidth="35920" windowHeight="20800" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="1950" yWindow="795" windowWidth="44835" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="195">
   <si>
     <t>*N/A*</t>
   </si>
@@ -615,6 +615,12 @@
   </si>
   <si>
     <t>&lt;a href='https://academic.oup.com/jogss/pages/General_Instructions'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>State Politics &amp; Policy Quarterly</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/state-politics-and-policy-quarterly'target='_blank'&gt;Short Article&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -986,21 +992,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="2" max="2" width="135.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="135.375" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1392,7 +1398,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>182</v>
       </c>
@@ -1434,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1448,7 +1454,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1462,7 +1468,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1476,7 +1482,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -1546,7 +1552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>176</v>
       </c>
@@ -1560,7 +1566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1630,7 +1636,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1672,7 +1678,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1686,7 +1692,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1700,7 +1706,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1728,7 +1734,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1770,7 +1776,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1784,7 +1790,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1812,7 +1818,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1826,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1854,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -1896,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>180</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -1924,7 +1930,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>186</v>
       </c>
@@ -1938,7 +1944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>191</v>
       </c>
@@ -1964,6 +1970,20 @@
       </c>
       <c r="D69">
         <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removes a duplicate from notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2008722D-8A2D-4A31-8080-3248B042069E}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53D4ACF7-11C0-4D4B-8832-E0921FE3565C}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="795" windowWidth="44835" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="194">
   <si>
     <t>*N/A*</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=rpgi20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=rpgi20#prep'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
   <si>
     <t>&lt;a href='https://academic.oup.com/afraf/pages/research_notes'target='_blank'&gt;Research Note&lt;/a&gt;</t>
@@ -992,21 +989,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
-    <col min="2" max="2" width="135.375" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="135.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +1015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1028,13 +1023,13 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
         <v>120</v>
       </c>
-      <c r="D2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1042,13 +1037,13 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" t="s">
         <v>122</v>
       </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1056,13 +1051,13 @@
         <v>65</v>
       </c>
       <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
         <v>124</v>
       </c>
-      <c r="D4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1070,13 +1065,13 @@
         <v>66</v>
       </c>
       <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
         <v>126</v>
       </c>
-      <c r="D5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1084,13 +1079,13 @@
         <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1098,41 +1093,41 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" t="s">
         <v>128</v>
       </c>
-      <c r="D7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s">
         <v>172</v>
       </c>
-      <c r="B8" t="s">
-        <v>173</v>
-      </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
         <v>174</v>
       </c>
-      <c r="B9" t="s">
-        <v>175</v>
-      </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1140,13 +1135,13 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" t="s">
         <v>130</v>
       </c>
-      <c r="D10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1154,13 +1149,13 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1168,13 +1163,13 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1182,13 +1177,13 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1196,13 +1191,13 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" t="s">
         <v>134</v>
       </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1210,13 +1205,13 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1224,13 +1219,13 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" t="s">
         <v>136</v>
       </c>
-      <c r="D16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1238,13 +1233,13 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1252,13 +1247,13 @@
         <v>77</v>
       </c>
       <c r="C18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" t="s">
         <v>139</v>
       </c>
-      <c r="D18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1266,13 +1261,13 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1280,13 +1275,13 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1294,13 +1289,13 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1308,13 +1303,13 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1322,55 +1317,55 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" t="s">
         <v>143</v>
       </c>
-      <c r="D23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>84</v>
       </c>
       <c r="C25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" t="s">
         <v>145</v>
       </c>
-      <c r="D25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1378,617 +1373,603 @@
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>87</v>
       </c>
       <c r="C28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" t="s">
         <v>148</v>
       </c>
-      <c r="D28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
         <v>89</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>150</v>
       </c>
-      <c r="D30" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>182</v>
-      </c>
-      <c r="B31" t="s">
-        <v>183</v>
-      </c>
-      <c r="C31" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>90</v>
       </c>
       <c r="C32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" t="s">
         <v>151</v>
       </c>
-      <c r="D32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>94</v>
       </c>
       <c r="C36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" t="s">
         <v>155</v>
       </c>
-      <c r="D36" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
         <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>175</v>
+      </c>
+      <c r="B39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" t="s">
-        <v>179</v>
-      </c>
-      <c r="C39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>98</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D42" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D43" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>102</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D46" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>105</v>
       </c>
       <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
         <v>161</v>
       </c>
-      <c r="D49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="D51" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D53" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="D55" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D56" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>114</v>
       </c>
       <c r="C58" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>115</v>
       </c>
       <c r="C59" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="D59" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="D60" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>117</v>
       </c>
       <c r="C61" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="D61" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D62" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>2</v>
+        <v>179</v>
       </c>
       <c r="B64" t="s">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B65" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
-      </c>
-      <c r="D65" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D65">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" t="s">
+        <v>189</v>
+      </c>
+      <c r="C67" t="s">
+        <v>188</v>
+      </c>
+      <c r="D67">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>186</v>
-      </c>
-      <c r="B67" t="s">
-        <v>187</v>
-      </c>
-      <c r="C67" t="s">
-        <v>128</v>
-      </c>
-      <c r="D67">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>188</v>
-      </c>
-      <c r="B68" t="s">
-        <v>190</v>
-      </c>
-      <c r="C68" t="s">
-        <v>189</v>
-      </c>
-      <c r="D68">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B69" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D69">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>193</v>
-      </c>
-      <c r="B70" t="s">
-        <v>194</v>
-      </c>
-      <c r="C70" t="s">
-        <v>120</v>
-      </c>
-      <c r="D70">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">
-    <sortCondition descending="1" ref="D2:D58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
+    <sortCondition descending="1" ref="D2:D57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds several journals to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53D4ACF7-11C0-4D4B-8832-E0921FE3565C}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237130B9-286F-084B-9AF9-396CAE129DE1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="211">
   <si>
     <t>*N/A*</t>
   </si>
@@ -239,9 +239,6 @@
     <t>&lt;a href='https://www.cambridge.org/core/journals/international-organization/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=fwep20#Preparing_your_paper'target='_blank'&gt;Research Note&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://ejpr.onlinelibrary.wiley.com/hub/journal/14756765/homepage/forauthors.html'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
   <si>
@@ -314,15 +311,9 @@
     <t>&lt;a href='https://www.frontiersin.org/journals/political-science/for-authors/article-types'target='_blank'&gt;Brief Research Report&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?journalCode=fbep20&amp;page=instructions#prep'target='_blank'&gt;Research Note&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.cambridge.org/core/journals/journal-of-experimental-political-science/information/author-instructions/preparing-your-materials'target='_blank'&gt;Short Report&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?journalCode=rrep20&amp;page=instructions'target='_blank'&gt;Research Note&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.cambridge.org/core/journals/canadian-journal-of-political-science-revue-canadienne-de-science-politique/information/instructions-for-contributors-directives-aux-auteurs-es'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
   <si>
@@ -365,12 +356,6 @@
     <t>&lt;a href='https://brazilianpoliticalsciencereview.org/author-guidelines/'target='_blank'&gt;Research in Progress&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?journalCode=fjls20&amp;page=instructions#Word_limits'target='_blank'&gt;Research Note&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=fips20#article-types'target='_blank'&gt;Note&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://onlinelibrary.wiley.com/page/journal/14679477/homepage/forauthors.html'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
   <si>
@@ -389,9 +374,6 @@
     <t>&lt;a href='https://brill.com/view/journals/parl/parl-overview.xml'target='_blank'&gt;Report&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=prxx20#prep'target='_blank'&gt;Research Note&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=rpnz20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
   <si>
@@ -618,14 +600,91 @@
   </si>
   <si>
     <t>&lt;a href='https://www.cambridge.org/core/journals/state-politics-and-policy-quarterly'target='_blank'&gt;Short Article&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Political Studies</t>
+  </si>
+  <si>
+    <t>Philosophy and Public Affairs</t>
+  </si>
+  <si>
+    <t>European Political Science Review</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/european-political-science-review'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Publius: The Journal of Federalism</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://academic.oup.com/publius'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://journals.sagepub.com/author-instructions/POL'target='_blank'&gt;Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://journals.sagepub.com/author-instructions/PSX'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://onlinelibrary.wiley.com/page/journal/10884963/homepage/forauthors.html'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=fbep20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=fjls20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=rrep20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=fips20'target='_blank'&gt;Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=fwep20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=prxx20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Politica y Gobierno</t>
+  </si>
+  <si>
+    <t>&lt;a href='http://www.politicaygobierno.cide.edu/index.php/pyg/tipo_envios'target='_blank'&gt;Nota de investigación&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>9k words</t>
+  </si>
+  <si>
+    <t>Journal of Law and Courts</t>
+  </si>
+  <si>
+    <t>Journal of Race, Ethnicity, and Politics</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/journal-of-law-and-courts/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/journal-of-race-ethnicity-and-politics/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -653,8 +712,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -989,9 +1052,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1002,266 +1067,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" t="s">
-        <v>126</v>
+        <v>182</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>173</v>
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D9">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
         <v>139</v>
@@ -1269,181 +1334,181 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>27</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>195</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>144</v>
-      </c>
-      <c r="D24" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+      <c r="D24">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>30</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" t="s">
-        <v>145</v>
+        <v>132</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30">
-        <v>29</v>
+        <v>125</v>
+      </c>
+      <c r="D30" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D32" t="s">
         <v>151</v>
@@ -1451,525 +1516,637 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D33" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D35" t="s">
-        <v>155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D36" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>175</v>
+        <v>129</v>
+      </c>
+      <c r="D38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="D39">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" t="s">
-        <v>157</v>
+        <v>121</v>
+      </c>
+      <c r="D42">
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>186</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
-      </c>
-      <c r="D46" t="s">
-        <v>159</v>
+        <v>113</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>173</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
-      </c>
-      <c r="D52" t="s">
-        <v>164</v>
+        <v>143</v>
+      </c>
+      <c r="D52">
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="D54" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>169</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" t="s">
-        <v>167</v>
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C57" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="C58" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58" t="s">
-        <v>0</v>
+        <v>113</v>
+      </c>
+      <c r="D58">
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>170</v>
+        <v>113</v>
       </c>
       <c r="D60" t="s">
-        <v>0</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="C61" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D61" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D62" t="s">
-        <v>0</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>0</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>179</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>180</v>
+        <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="D64" t="s">
-        <v>0</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
-      </c>
-      <c r="D65">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>185</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="C66" t="s">
-        <v>127</v>
-      </c>
-      <c r="D66">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>187</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
-        <v>188</v>
-      </c>
-      <c r="D67">
-        <v>18</v>
+        <v>113</v>
+      </c>
+      <c r="D67" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>131</v>
-      </c>
-      <c r="D68">
-        <v>28</v>
+        <v>129</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C69" t="s">
-        <v>119</v>
-      </c>
-      <c r="D69">
-        <v>17</v>
+        <v>121</v>
+      </c>
+      <c r="D69" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" t="s">
+        <v>121</v>
+      </c>
+      <c r="D72" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" t="s">
+        <v>121</v>
+      </c>
+      <c r="D73">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>204</v>
+      </c>
+      <c r="B75" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B76" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>208</v>
+      </c>
+      <c r="B77" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" t="s">
+        <v>125</v>
+      </c>
+      <c r="D77">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
-    <sortCondition descending="1" ref="D2:D57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D74">
+    <sortCondition ref="B1:B74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds AustralianJPS to notes
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237130B9-286F-084B-9AF9-396CAE129DE1}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519F0A2F-B86B-C745-9222-7C56DAD0FB3E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="17640" yWindow="500" windowWidth="30240" windowHeight="17180" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="213">
   <si>
     <t>*N/A*</t>
   </si>
@@ -669,6 +669,12 @@
   </si>
   <si>
     <t>&lt;a href='https://www.cambridge.org/core/journals/journal-of-race-ethnicity-and-politics/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Australian Journal of Political Science</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=cajp20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2144,6 +2150,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>211</v>
+      </c>
+      <c r="B78" t="s">
+        <v>212</v>
+      </c>
+      <c r="C78" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D74">
     <sortCondition ref="B1:B74"/>

</xml_diff>

<commit_message>
removes exact date up last update
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519F0A2F-B86B-C745-9222-7C56DAD0FB3E}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA46423D-3823-064A-BEDD-E75D95554772}"/>
   <bookViews>
-    <workbookView xWindow="17640" yWindow="500" windowWidth="30240" windowHeight="17180" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="9100" yWindow="500" windowWidth="38780" windowHeight="17180" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="218">
   <si>
     <t>*N/A*</t>
   </si>
@@ -675,6 +675,21 @@
   </si>
   <si>
     <t>&lt;a href='https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=cajp20'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Nationalities Papers</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/nationalities-papers/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Politics and Religion</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/politics-and-religion/information/author-instructions/preparing-your-materials'target='_blank'&gt;Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>4.5k words</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,6 +2179,34 @@
         <v>17</v>
       </c>
     </row>
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" t="s">
+        <v>214</v>
+      </c>
+      <c r="C79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B80" t="s">
+        <v>216</v>
+      </c>
+      <c r="C80" t="s">
+        <v>217</v>
+      </c>
+      <c r="D80">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D74">
     <sortCondition ref="B1:B74"/>

</xml_diff>

<commit_message>
apsr research notes added
</commit_message>
<xml_diff>
--- a/content/blog/data/research_notes.xlsx
+++ b/content/blog/data/research_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/phwc76_durham_ac_uk/Documents/websites/resulumit.com/content/blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07530D1C-F823-43B7-AF13-08B0FA532A2E}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="8_{E8096AAE-1289-4D57-BFE8-FA76B2E6C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F66D91C3-583A-1043-8548-5EDFB2931031}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="75" windowWidth="42180" windowHeight="20805" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
+    <workbookView xWindow="7360" yWindow="500" windowWidth="42180" windowHeight="20800" xr2:uid="{A2E98F91-3A7E-ED47-92F6-C8E64A4C00D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="210">
   <si>
     <t>5k -- 8k words</t>
   </si>
@@ -657,6 +657,15 @@
   </si>
   <si>
     <t>&lt;a href='https://www.journals.uchicago.edu/journals/apt/instruct'target='_blank'&gt;Research Note&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>American Political Science Review</t>
+  </si>
+  <si>
+    <t>7k words</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cambridge.org/core/journals/american-political-science-review/information/author-instructions/preparing-your-materials'target='_blank'&gt;Research Note&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1040,21 +1049,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7077210-50C0-314B-8951-9DBEC2D4D539}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="135.375" customWidth="1"/>
+    <col min="3" max="3" width="135.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1110,7 +1119,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -1166,7 +1175,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1208,7 +1217,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1222,7 +1231,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1264,7 +1273,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -1278,7 +1287,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1306,7 +1315,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1320,7 +1329,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1362,7 +1371,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>199</v>
       </c>
@@ -1376,7 +1385,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1390,7 +1399,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>157</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1441,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1460,7 +1469,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>142</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -1530,7 +1539,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1544,7 +1553,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>144</v>
       </c>
@@ -1558,7 +1567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1572,7 +1581,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>144</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1600,7 +1609,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>197</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>138</v>
       </c>
@@ -1642,7 +1651,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -1656,7 +1665,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>180</v>
       </c>
@@ -1698,7 +1707,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>159</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>136</v>
       </c>
@@ -1737,7 +1746,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -1765,7 +1774,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -1779,7 +1788,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -1793,7 +1802,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -1807,7 +1816,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -1821,7 +1830,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -1835,7 +1844,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>182</v>
       </c>
@@ -1849,7 +1858,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>46</v>
       </c>
@@ -1874,7 +1883,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>190</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -1902,7 +1911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -1916,7 +1925,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>175</v>
       </c>
@@ -1930,7 +1939,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>192</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -1958,7 +1967,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>178</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>50</v>
       </c>
@@ -1986,7 +1995,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -2000,7 +2009,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -2014,7 +2023,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>52</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>53</v>
       </c>
@@ -2042,7 +2051,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>203</v>
       </c>
@@ -2056,7 +2065,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>146</v>
       </c>
@@ -2070,7 +2079,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>54</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -2098,7 +2107,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -2112,7 +2121,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>194</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>188</v>
       </c>
@@ -2140,7 +2149,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>205</v>
       </c>
@@ -2154,7 +2163,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -2165,7 +2174,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>58</v>
       </c>
@@ -2176,7 +2185,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>161</v>
       </c>
@@ -2187,7 +2196,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>156</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>56</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>140</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -2228,7 +2237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>59</v>
       </c>
@@ -2239,7 +2248,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>60</v>
       </c>
@@ -2250,7 +2259,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>174</v>
       </c>
@@ -2258,12 +2267,26 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>201</v>
       </c>
       <c r="C90" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>207</v>
+      </c>
+      <c r="B91">
+        <v>82</v>
+      </c>
+      <c r="C91" t="s">
+        <v>209</v>
+      </c>
+      <c r="D91" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>